<commit_message>
Rewrite simulation code as functions.
</commit_message>
<xml_diff>
--- a/Test for Equality of Variances Simulation Results.xlsx
+++ b/Test for Equality of Variances Simulation Results.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Judy Zhang\Documents\Academics\2021-2022\Fall2021\Research Group\Papers\Paper by Topics\Detect Difference in Variances\Test Power\Power of F Test\PowerCalculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B605027-8631-4169-A952-D2729EBF533C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18915DB4-4393-4B0F-BAD0-391C1C13A374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sim1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Parameters</t>
   </si>
@@ -36,9 +45,6 @@
     <t>Treatment Group</t>
   </si>
   <si>
-    <t>Population Size (N)</t>
-  </si>
-  <si>
     <t>Sample Size (n)</t>
   </si>
   <si>
@@ -48,9 +54,6 @@
     <t>Population Mean</t>
   </si>
   <si>
-    <t>10^2</t>
-  </si>
-  <si>
     <t>Statistical Test</t>
   </si>
   <si>
@@ -63,12 +66,6 @@
     <t>Significance Level (alpha)</t>
   </si>
   <si>
-    <t>Sample Mean (x_bar)</t>
-  </si>
-  <si>
-    <t>Sample Variance (s^2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test Statistic </t>
   </si>
   <si>
@@ -81,12 +78,6 @@
     <t>Critical Value</t>
   </si>
   <si>
-    <t>p-Value</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>Type I Error Rate</t>
   </si>
   <si>
@@ -94,6 +85,57 @@
   </si>
   <si>
     <t>Total Number of Simulations:</t>
+  </si>
+  <si>
+    <t>Population Distribution</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Normal (Standard)</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>sX^2</t>
+  </si>
+  <si>
+    <t>sY^2</t>
+  </si>
+  <si>
+    <t>Sample Mean</t>
+  </si>
+  <si>
+    <t>x_bar</t>
+  </si>
+  <si>
+    <t>y_bar</t>
+  </si>
+  <si>
+    <t>F = sX^2/sY^2</t>
+  </si>
+  <si>
+    <t>F_30-1,30-1</t>
+  </si>
+  <si>
+    <t>F_30-1,30-1(ncp = 0+0)</t>
+  </si>
+  <si>
+    <t>F_1-0.05/2, 30-1, 30-1 and F_0.05/2, 30-1, 30-1 (Two)</t>
+  </si>
+  <si>
+    <t>F_0.05, 30-1, 30-1 (Lower)</t>
+  </si>
+  <si>
+    <t>F_1-0.05, 30-1, 30-1 (Upper)</t>
+  </si>
+  <si>
+    <t>Theoretical Power</t>
+  </si>
+  <si>
+    <t>Empirical Power</t>
   </si>
 </sst>
 </file>
@@ -438,7 +480,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,127 +505,168 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B7" s="2">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+      <c r="B17" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.05</v>
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.05</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="B35" s="2">
+        <f>1233/10000</f>
+        <v>0.12330000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>